<commit_message>
dashboard  turnover chart done and bug correction
</commit_message>
<xml_diff>
--- a/Stock.xlsx
+++ b/Stock.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Barcode</t>
   </si>
@@ -32,55 +32,34 @@
     <t xml:space="preserve">Expiration Date </t>
   </si>
   <si>
-    <t>123</t>
+    <t>1</t>
   </si>
   <si>
-    <t>chips mahboul gout barbecue</t>
+    <t>PC</t>
   </si>
   <si>
-    <t>21</t>
+    <t>10</t>
   </si>
   <si>
-    <t>1</t>
+    <t>2000</t>
+  </si>
+  <si>
+    <t>3000</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Tomate</t>
+  </si>
+  <si>
+    <t>100</t>
   </si>
   <si>
     <t>12</t>
   </si>
   <si>
-    <t>2020-05-09</t>
-  </si>
-  <si>
-    <t>gedila</t>
-  </si>
-  <si>
-    <t>872</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>27</t>
-  </si>
-  <si>
-    <t>2020-05-12</t>
-  </si>
-  <si>
-    <t>MA3DNOUS</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>Zit Zitoune</t>
-  </si>
-  <si>
-    <t>23</t>
+    <t>2020-05-31</t>
   </si>
 </sst>
 </file>
@@ -125,7 +104,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -167,13 +146,11 @@
       <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
+      <c r="F2"/>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
@@ -182,53 +159,13 @@
         <v>13</v>
       </c>
       <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
         <v>14</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>15</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dashboard areachart and piechart done with tabpane
</commit_message>
<xml_diff>
--- a/Stock.xlsx
+++ b/Stock.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Barcode</t>
   </si>
@@ -38,7 +38,7 @@
     <t>PC</t>
   </si>
   <si>
-    <t>10</t>
+    <t>4</t>
   </si>
   <si>
     <t>2000</t>
@@ -53,7 +53,10 @@
     <t>Tomate</t>
   </si>
   <si>
-    <t>100</t>
+    <t>95</t>
+  </si>
+  <si>
+    <t>10</t>
   </si>
   <si>
     <t>12</t>
@@ -159,13 +162,13 @@
         <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>